<commit_message>
Update performance dashboard 2025-12-19 00:32
</commit_message>
<xml_diff>
--- a/performance-dashboard/archive/Trading_Performance_20251219.xlsx
+++ b/performance-dashboard/archive/Trading_Performance_20251219.xlsx
@@ -599,27 +599,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>¥771,708.00</t>
+          <t>¥1,000,000.00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>¥724,239.00</t>
+          <t>¥1,001,002.00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>¥-47,469.00</t>
+          <t>¥+1,002.00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>-6.15%</t>
+          <t>+0.10%</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>-100.00%</t>
+          <t>+28.71%</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -627,17 +627,17 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>6.15%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>-6.1512%</t>
+          <t>0.1002%</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -1790,27 +1790,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>¥771,708.00</t>
+          <t>¥1,000,000.00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>¥724,239.00</t>
+          <t>¥1,001,002.00</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>¥-47,469.00</t>
+          <t>¥+1,002.00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>-6.15%</t>
+          <t>+0.10%</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>-100.00%</t>
+          <t>+28.71%</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -1818,17 +1818,17 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>6.15%</t>
+          <t>0.00%</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>-6.1512%</t>
+          <t>0.1002%</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">

</xml_diff>